<commit_message>
Update Base de Datos Oficial.xlsx
prueba
</commit_message>
<xml_diff>
--- a/Base de Datos Oficial.xlsx
+++ b/Base de Datos Oficial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcoyo\Documents\GitHub\Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CB75EF-BB15-4C2E-B7BC-789B7B0851C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58135678-0D6E-40DF-91BC-CCE2147AD154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="45" windowWidth="14400" windowHeight="8685" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="465" yWindow="45" windowWidth="14400" windowHeight="8685" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS_NOMBRESLARGOS" sheetId="1" r:id="rId1"/>
@@ -987,7 +987,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>Periodo</t>
   </si>
@@ -1086,6 +1086,9 @@
   </si>
   <si>
     <t>tasa_IPC_acum</t>
+  </si>
+  <si>
+    <t>Pauli linda</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1487,6 +1490,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -49492,7 +49496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC272FD2-5EC4-4BE4-878F-346441666433}">
   <dimension ref="A1:J145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView topLeftCell="A139" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -54153,10 +54157,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EA5142-E3F9-4F44-9674-B41C6DD2952D}">
-  <dimension ref="B1:G15"/>
+  <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54444,6 +54448,11 @@
       </c>
       <c r="G15" s="35"/>
     </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="39" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
@@ -54453,9 +54462,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54623,19 +54635,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD324055-1338-4DF6-8FEE-42FB9AAA38D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD32C1C-3DB8-4C8D-B863-300A0DFAA3C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -54659,9 +54667,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD32C1C-3DB8-4C8D-B863-300A0DFAA3C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD324055-1338-4DF6-8FEE-42FB9AAA38D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>